<commit_message>
0.3.2 - Trainee Assignments bug fixed. Trainees name visible now.
</commit_message>
<xml_diff>
--- a/keel_cadet_import_template.xlsx
+++ b/keel_cadet_import_template.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29426"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9E8ED2F5-90C4-4007-B44D-01C92958DA94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B5DF211-4263-4294-A025-0D441711C069}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="602">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="599">
   <si>
     <t>Full Name</t>
   </si>
@@ -978,9 +978,6 @@
     <t>S12345</t>
   </si>
   <si>
-    <t>DECK_CADET</t>
-  </si>
-  <si>
     <t>Sarah Jenkins</t>
   </si>
   <si>
@@ -1065,9 +1062,6 @@
     <t>S77665</t>
   </si>
   <si>
-    <t>ENGINE_CADET</t>
-  </si>
-  <si>
     <t>Liam O'Connor</t>
   </si>
   <si>
@@ -1141,9 +1135,6 @@
   </si>
   <si>
     <t>S33445</t>
-  </si>
-  <si>
-    <t>ETO_CADET</t>
   </si>
   <si>
     <t>David Chen</t>
@@ -2214,7 +2205,7 @@
   <dimension ref="A1:AC26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="Z29" sqref="Z29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2412,7 +2403,7 @@
         <v>319</v>
       </c>
       <c r="AA2" t="s">
-        <v>320</v>
+        <v>32</v>
       </c>
       <c r="AB2" s="2">
         <v>45306</v>
@@ -2423,31 +2414,31 @@
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B3" s="2">
         <v>37854</v>
       </c>
       <c r="C3" t="s">
+        <v>321</v>
+      </c>
+      <c r="D3" t="s">
         <v>322</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>323</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>324</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>325</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>326</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>327</v>
-      </c>
-      <c r="I3" t="s">
-        <v>328</v>
       </c>
       <c r="J3">
         <v>4471234567</v>
@@ -2456,7 +2447,7 @@
         <v>30</v>
       </c>
       <c r="L3" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="M3" t="s">
         <v>36</v>
@@ -2465,13 +2456,13 @@
         <v>4471112222</v>
       </c>
       <c r="O3" t="s">
+        <v>329</v>
+      </c>
+      <c r="P3" t="s">
         <v>330</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>331</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>332</v>
       </c>
       <c r="R3" s="2">
         <v>44336</v>
@@ -2480,13 +2471,13 @@
         <v>47987</v>
       </c>
       <c r="T3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="U3" t="s">
+        <v>332</v>
+      </c>
+      <c r="V3" t="s">
         <v>333</v>
-      </c>
-      <c r="V3" t="s">
-        <v>334</v>
       </c>
       <c r="W3" s="2">
         <v>44357</v>
@@ -2495,13 +2486,13 @@
         <v>48008</v>
       </c>
       <c r="Y3" t="s">
+        <v>334</v>
+      </c>
+      <c r="Z3" t="s">
         <v>335</v>
       </c>
-      <c r="Z3" t="s">
-        <v>336</v>
-      </c>
       <c r="AA3" t="s">
-        <v>320</v>
+        <v>37</v>
       </c>
       <c r="AB3" s="2">
         <v>45323</v>
@@ -2512,7 +2503,7 @@
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B4" s="2">
         <v>37198</v>
@@ -2521,22 +2512,22 @@
         <v>307</v>
       </c>
       <c r="D4" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E4" t="s">
         <v>309</v>
       </c>
       <c r="F4" t="s">
+        <v>338</v>
+      </c>
+      <c r="G4" t="s">
         <v>339</v>
-      </c>
-      <c r="G4" t="s">
-        <v>340</v>
       </c>
       <c r="H4">
         <v>122001</v>
       </c>
       <c r="I4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="J4">
         <v>9910055443</v>
@@ -2545,7 +2536,7 @@
         <v>40</v>
       </c>
       <c r="L4" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="M4" t="s">
         <v>36</v>
@@ -2554,10 +2545,10 @@
         <v>9910011223</v>
       </c>
       <c r="O4" t="s">
+        <v>342</v>
+      </c>
+      <c r="P4" t="s">
         <v>343</v>
-      </c>
-      <c r="P4" t="s">
-        <v>344</v>
       </c>
       <c r="Q4" t="s">
         <v>316</v>
@@ -2569,10 +2560,10 @@
         <v>47556</v>
       </c>
       <c r="T4" t="s">
+        <v>344</v>
+      </c>
+      <c r="U4" t="s">
         <v>345</v>
-      </c>
-      <c r="U4" t="s">
-        <v>346</v>
       </c>
       <c r="V4" t="s">
         <v>156</v>
@@ -2584,13 +2575,13 @@
         <v>47573</v>
       </c>
       <c r="Y4" t="s">
+        <v>346</v>
+      </c>
+      <c r="Z4" t="s">
         <v>347</v>
       </c>
-      <c r="Z4" t="s">
-        <v>348</v>
-      </c>
       <c r="AA4" t="s">
-        <v>349</v>
+        <v>42</v>
       </c>
       <c r="AB4" s="2">
         <v>45306</v>
@@ -2601,7 +2592,7 @@
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B5" s="2">
         <v>37281</v>
@@ -2610,22 +2601,22 @@
         <v>307</v>
       </c>
       <c r="D5" t="s">
+        <v>349</v>
+      </c>
+      <c r="E5" t="s">
+        <v>350</v>
+      </c>
+      <c r="F5" t="s">
         <v>351</v>
       </c>
-      <c r="E5" t="s">
+      <c r="G5" t="s">
         <v>352</v>
       </c>
-      <c r="F5" t="s">
+      <c r="H5" t="s">
         <v>353</v>
       </c>
-      <c r="G5" t="s">
+      <c r="I5" t="s">
         <v>354</v>
-      </c>
-      <c r="H5" t="s">
-        <v>355</v>
-      </c>
-      <c r="I5" t="s">
-        <v>356</v>
       </c>
       <c r="J5">
         <v>353851234</v>
@@ -2634,7 +2625,7 @@
         <v>60</v>
       </c>
       <c r="L5" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="M5" t="s">
         <v>31</v>
@@ -2643,13 +2634,13 @@
         <v>353859999</v>
       </c>
       <c r="O5" t="s">
+        <v>356</v>
+      </c>
+      <c r="P5" t="s">
+        <v>357</v>
+      </c>
+      <c r="Q5" t="s">
         <v>358</v>
-      </c>
-      <c r="P5" t="s">
-        <v>359</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>360</v>
       </c>
       <c r="R5" s="2">
         <v>45181</v>
@@ -2658,10 +2649,10 @@
         <v>48833</v>
       </c>
       <c r="T5" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="U5" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="V5" t="s">
         <v>160</v>
@@ -2673,13 +2664,13 @@
         <v>48852</v>
       </c>
       <c r="Y5" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="Z5" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="AA5" t="s">
-        <v>320</v>
+        <v>46</v>
       </c>
       <c r="AB5" s="2">
         <v>45361</v>
@@ -2690,31 +2681,31 @@
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B6" s="2">
         <v>37969</v>
       </c>
       <c r="C6" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D6" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="E6" t="s">
         <v>309</v>
       </c>
       <c r="F6" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="G6" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="H6">
         <v>600002</v>
       </c>
       <c r="I6" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="J6">
         <v>9444012345</v>
@@ -2723,7 +2714,7 @@
         <v>35</v>
       </c>
       <c r="L6" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="M6" t="s">
         <v>31</v>
@@ -2732,10 +2723,10 @@
         <v>9444055555</v>
       </c>
       <c r="O6" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="P6" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="Q6" t="s">
         <v>316</v>
@@ -2747,10 +2738,10 @@
         <v>48522</v>
       </c>
       <c r="T6" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="U6" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="V6" t="s">
         <v>156</v>
@@ -2762,13 +2753,13 @@
         <v>48548</v>
       </c>
       <c r="Y6" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="Z6" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="AA6" t="s">
-        <v>375</v>
+        <v>50</v>
       </c>
       <c r="AB6" s="2">
         <v>45337</v>
@@ -2779,7 +2770,7 @@
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="B7" s="2">
         <v>37102</v>
@@ -2788,13 +2779,13 @@
         <v>307</v>
       </c>
       <c r="D7" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="E7" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="F7" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="G7" t="s">
         <v>254</v>
@@ -2803,7 +2794,7 @@
         <v>238884</v>
       </c>
       <c r="I7" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="J7">
         <v>659123456</v>
@@ -2812,7 +2803,7 @@
         <v>44</v>
       </c>
       <c r="L7" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="M7" t="s">
         <v>36</v>
@@ -2821,13 +2812,13 @@
         <v>659111222</v>
       </c>
       <c r="O7" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="P7" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="Q7" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="R7" s="2">
         <v>43845</v>
@@ -2839,7 +2830,7 @@
         <v>254</v>
       </c>
       <c r="U7" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="V7" t="s">
         <v>254</v>
@@ -2851,13 +2842,13 @@
         <v>47514</v>
       </c>
       <c r="Y7" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="Z7" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="AA7" t="s">
-        <v>320</v>
+        <v>54</v>
       </c>
       <c r="AB7" s="2">
         <v>45311</v>
@@ -2868,7 +2859,7 @@
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="B8" s="2">
         <v>37351</v>
@@ -2877,22 +2868,22 @@
         <v>307</v>
       </c>
       <c r="D8" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="E8" t="s">
         <v>309</v>
       </c>
       <c r="F8" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="G8" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="H8">
         <v>700091</v>
       </c>
       <c r="I8" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="J8">
         <v>9830055667</v>
@@ -2901,7 +2892,7 @@
         <v>48</v>
       </c>
       <c r="L8" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="M8" t="s">
         <v>31</v>
@@ -2910,10 +2901,10 @@
         <v>9830011223</v>
       </c>
       <c r="O8" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="P8" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="Q8" t="s">
         <v>316</v>
@@ -2925,10 +2916,10 @@
         <v>48079</v>
       </c>
       <c r="T8" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="U8" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="V8" t="s">
         <v>156</v>
@@ -2940,13 +2931,13 @@
         <v>48100</v>
       </c>
       <c r="Y8" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="Z8" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="AA8" t="s">
-        <v>320</v>
+        <v>58</v>
       </c>
       <c r="AB8" s="2">
         <v>45352</v>
@@ -2957,31 +2948,31 @@
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="B9" s="2">
         <v>37517</v>
       </c>
       <c r="C9" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D9" t="s">
+        <v>395</v>
+      </c>
+      <c r="E9" t="s">
+        <v>396</v>
+      </c>
+      <c r="F9" t="s">
+        <v>397</v>
+      </c>
+      <c r="G9" t="s">
         <v>398</v>
-      </c>
-      <c r="E9" t="s">
-        <v>399</v>
-      </c>
-      <c r="F9" t="s">
-        <v>400</v>
-      </c>
-      <c r="G9" t="s">
-        <v>401</v>
       </c>
       <c r="H9">
         <v>184</v>
       </c>
       <c r="I9" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="J9">
         <v>393331234</v>
@@ -2990,7 +2981,7 @@
         <v>56</v>
       </c>
       <c r="L9" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="M9" t="s">
         <v>31</v>
@@ -2999,13 +2990,13 @@
         <v>393339999</v>
       </c>
       <c r="O9" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="P9" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="Q9" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="R9" s="2">
         <v>44936</v>
@@ -3014,10 +3005,10 @@
         <v>48588</v>
       </c>
       <c r="T9" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="U9" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="V9" t="s">
         <v>162</v>
@@ -3029,13 +3020,13 @@
         <v>48610</v>
       </c>
       <c r="Y9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="Z9" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="AA9" t="s">
-        <v>320</v>
+        <v>32</v>
       </c>
       <c r="AB9" s="2">
         <v>45342</v>
@@ -3046,7 +3037,7 @@
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="B10" s="2">
         <v>36950</v>
@@ -3055,22 +3046,22 @@
         <v>307</v>
       </c>
       <c r="D10" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="E10" t="s">
         <v>309</v>
       </c>
       <c r="F10" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="G10" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="H10">
         <v>682001</v>
       </c>
       <c r="I10" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="J10">
         <v>9447011223</v>
@@ -3079,7 +3070,7 @@
         <v>30</v>
       </c>
       <c r="L10" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="M10" t="s">
         <v>31</v>
@@ -3088,10 +3079,10 @@
         <v>9447055667</v>
       </c>
       <c r="O10" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="P10" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="Q10" t="s">
         <v>316</v>
@@ -3103,10 +3094,10 @@
         <v>47821</v>
       </c>
       <c r="T10" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="U10" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="V10" t="s">
         <v>156</v>
@@ -3118,13 +3109,13 @@
         <v>47848</v>
       </c>
       <c r="Y10" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="Z10" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="AA10" t="s">
-        <v>349</v>
+        <v>37</v>
       </c>
       <c r="AB10" s="2">
         <v>45306</v>
@@ -3135,7 +3126,7 @@
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="B11" s="2">
         <v>37691</v>
@@ -3144,22 +3135,22 @@
         <v>307</v>
       </c>
       <c r="D11" t="s">
+        <v>418</v>
+      </c>
+      <c r="E11" t="s">
+        <v>419</v>
+      </c>
+      <c r="F11" t="s">
+        <v>420</v>
+      </c>
+      <c r="G11" t="s">
         <v>421</v>
-      </c>
-      <c r="E11" t="s">
-        <v>422</v>
-      </c>
-      <c r="F11" t="s">
-        <v>423</v>
-      </c>
-      <c r="G11" t="s">
-        <v>424</v>
       </c>
       <c r="H11">
         <v>10115</v>
       </c>
       <c r="I11" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="J11">
         <v>491512345</v>
@@ -3168,7 +3159,7 @@
         <v>40</v>
       </c>
       <c r="L11" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="M11" t="s">
         <v>36</v>
@@ -3177,13 +3168,13 @@
         <v>491519999</v>
       </c>
       <c r="O11" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="P11" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="Q11" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="R11" s="2">
         <v>44663</v>
@@ -3192,10 +3183,10 @@
         <v>48315</v>
       </c>
       <c r="T11" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="U11" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="V11" t="s">
         <v>137</v>
@@ -3207,13 +3198,13 @@
         <v>48334</v>
       </c>
       <c r="Y11" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="Z11" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="AA11" t="s">
-        <v>320</v>
+        <v>42</v>
       </c>
       <c r="AB11" s="2">
         <v>45383</v>
@@ -3224,7 +3215,7 @@
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="B12" s="2">
         <v>37429</v>
@@ -3233,22 +3224,22 @@
         <v>307</v>
       </c>
       <c r="D12" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="E12" t="s">
         <v>309</v>
       </c>
       <c r="F12" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="G12" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="H12">
         <v>500033</v>
       </c>
       <c r="I12" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="J12">
         <v>9989012345</v>
@@ -3257,7 +3248,7 @@
         <v>60</v>
       </c>
       <c r="L12" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="M12" t="s">
         <v>36</v>
@@ -3266,10 +3257,10 @@
         <v>9989011111</v>
       </c>
       <c r="O12" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="P12" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="Q12" t="s">
         <v>316</v>
@@ -3281,10 +3272,10 @@
         <v>48135</v>
       </c>
       <c r="T12" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="U12" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="V12" t="s">
         <v>156</v>
@@ -3296,13 +3287,13 @@
         <v>48152</v>
       </c>
       <c r="Y12" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="Z12" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="AA12" t="s">
-        <v>320</v>
+        <v>46</v>
       </c>
       <c r="AB12" s="2">
         <v>45323</v>
@@ -3313,31 +3304,31 @@
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="B13" s="2">
         <v>37899</v>
       </c>
       <c r="C13" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D13" t="s">
+        <v>441</v>
+      </c>
+      <c r="E13" t="s">
+        <v>442</v>
+      </c>
+      <c r="F13" t="s">
+        <v>443</v>
+      </c>
+      <c r="G13" t="s">
         <v>444</v>
-      </c>
-      <c r="E13" t="s">
-        <v>445</v>
-      </c>
-      <c r="F13" t="s">
-        <v>446</v>
-      </c>
-      <c r="G13" t="s">
-        <v>447</v>
       </c>
       <c r="H13">
         <v>75001</v>
       </c>
       <c r="I13" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="J13">
         <v>336123456</v>
@@ -3346,7 +3337,7 @@
         <v>52</v>
       </c>
       <c r="L13" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="M13" t="s">
         <v>31</v>
@@ -3355,13 +3346,13 @@
         <v>336111222</v>
       </c>
       <c r="O13" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="P13" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="Q13" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="R13" s="2">
         <v>44762</v>
@@ -3370,10 +3361,10 @@
         <v>48414</v>
       </c>
       <c r="T13" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="U13" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="V13" t="s">
         <v>130</v>
@@ -3385,13 +3376,13 @@
         <v>48435</v>
       </c>
       <c r="Y13" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="Z13" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="AA13" t="s">
-        <v>320</v>
+        <v>50</v>
       </c>
       <c r="AB13" s="2">
         <v>45366</v>
@@ -3402,7 +3393,7 @@
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="B14" s="2">
         <v>37030</v>
@@ -3411,22 +3402,22 @@
         <v>307</v>
       </c>
       <c r="D14" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="E14" t="s">
         <v>309</v>
       </c>
       <c r="F14" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="G14" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="H14">
         <v>208001</v>
       </c>
       <c r="I14" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="J14">
         <v>9415012345</v>
@@ -3435,7 +3426,7 @@
         <v>30</v>
       </c>
       <c r="L14" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="M14" t="s">
         <v>31</v>
@@ -3444,10 +3435,10 @@
         <v>9415099887</v>
       </c>
       <c r="O14" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="P14" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="Q14" t="s">
         <v>316</v>
@@ -3459,10 +3450,10 @@
         <v>47704</v>
       </c>
       <c r="T14" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="U14" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="V14" t="s">
         <v>156</v>
@@ -3474,13 +3465,13 @@
         <v>47726</v>
       </c>
       <c r="Y14" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="Z14" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="AA14" t="s">
-        <v>349</v>
+        <v>54</v>
       </c>
       <c r="AB14" s="2">
         <v>45306</v>
@@ -3491,7 +3482,7 @@
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B15" s="2">
         <v>37591</v>
@@ -3500,22 +3491,22 @@
         <v>307</v>
       </c>
       <c r="D15" t="s">
+        <v>465</v>
+      </c>
+      <c r="E15" t="s">
+        <v>466</v>
+      </c>
+      <c r="F15" t="s">
+        <v>467</v>
+      </c>
+      <c r="G15" t="s">
         <v>468</v>
-      </c>
-      <c r="E15" t="s">
-        <v>469</v>
-      </c>
-      <c r="F15" t="s">
-        <v>470</v>
-      </c>
-      <c r="G15" t="s">
-        <v>471</v>
       </c>
       <c r="H15">
         <v>10005</v>
       </c>
       <c r="I15" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="J15">
         <v>121255501</v>
@@ -3524,7 +3515,7 @@
         <v>56</v>
       </c>
       <c r="L15" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="M15" t="s">
         <v>31</v>
@@ -3533,13 +3524,13 @@
         <v>121255502</v>
       </c>
       <c r="O15" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="P15" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="Q15" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="R15" s="2">
         <v>44242</v>
@@ -3548,13 +3539,13 @@
         <v>47893</v>
       </c>
       <c r="T15" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="U15" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="V15" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="W15" s="2">
         <v>44256</v>
@@ -3563,13 +3554,13 @@
         <v>47907</v>
       </c>
       <c r="Y15" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="Z15" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="AA15" t="s">
-        <v>320</v>
+        <v>58</v>
       </c>
       <c r="AB15" s="2">
         <v>45332</v>
@@ -3580,31 +3571,31 @@
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="B16" s="2">
         <v>37641</v>
       </c>
       <c r="C16" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D16" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="E16" t="s">
         <v>309</v>
       </c>
       <c r="F16" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="G16" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="H16">
         <v>141002</v>
       </c>
       <c r="I16" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="J16">
         <v>9814012345</v>
@@ -3613,7 +3604,7 @@
         <v>40</v>
       </c>
       <c r="L16" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="M16" t="s">
         <v>31</v>
@@ -3622,10 +3613,10 @@
         <v>9814099999</v>
       </c>
       <c r="O16" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="P16" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="Q16" t="s">
         <v>316</v>
@@ -3637,10 +3628,10 @@
         <v>48382</v>
       </c>
       <c r="T16" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="U16" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="V16" t="s">
         <v>156</v>
@@ -3652,13 +3643,13 @@
         <v>48404</v>
       </c>
       <c r="Y16" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="Z16" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="AA16" t="s">
-        <v>320</v>
+        <v>32</v>
       </c>
       <c r="AB16" s="2">
         <v>45397</v>
@@ -3669,7 +3660,7 @@
     </row>
     <row r="17" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="B17" s="2">
         <v>37159</v>
@@ -3678,22 +3669,22 @@
         <v>307</v>
       </c>
       <c r="D17" t="s">
+        <v>490</v>
+      </c>
+      <c r="E17" t="s">
+        <v>491</v>
+      </c>
+      <c r="F17" t="s">
+        <v>492</v>
+      </c>
+      <c r="G17" t="s">
         <v>493</v>
-      </c>
-      <c r="E17" t="s">
-        <v>494</v>
-      </c>
-      <c r="F17" t="s">
-        <v>495</v>
-      </c>
-      <c r="G17" t="s">
-        <v>496</v>
       </c>
       <c r="H17">
         <v>11511</v>
       </c>
       <c r="I17" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="J17">
         <v>201012345</v>
@@ -3702,7 +3693,7 @@
         <v>56</v>
       </c>
       <c r="L17" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="M17" t="s">
         <v>36</v>
@@ -3711,13 +3702,13 @@
         <v>201019999</v>
       </c>
       <c r="O17" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="P17" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="Q17" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="R17" s="2">
         <v>44147</v>
@@ -3726,10 +3717,10 @@
         <v>47798</v>
       </c>
       <c r="T17" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="U17" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="V17" t="s">
         <v>120</v>
@@ -3741,13 +3732,13 @@
         <v>47817</v>
       </c>
       <c r="Y17" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="Z17" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="AA17" t="s">
-        <v>320</v>
+        <v>37</v>
       </c>
       <c r="AB17" s="2">
         <v>45311</v>
@@ -3758,7 +3749,7 @@
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="B18" s="2">
         <v>37444</v>
@@ -3767,7 +3758,7 @@
         <v>307</v>
       </c>
       <c r="D18" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="E18" t="s">
         <v>309</v>
@@ -3776,13 +3767,13 @@
         <v>310</v>
       </c>
       <c r="G18" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="H18">
         <v>411001</v>
       </c>
       <c r="I18" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="J18">
         <v>9822012345</v>
@@ -3791,7 +3782,7 @@
         <v>35</v>
       </c>
       <c r="L18" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="M18" t="s">
         <v>36</v>
@@ -3800,10 +3791,10 @@
         <v>9822099887</v>
       </c>
       <c r="O18" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="P18" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="Q18" t="s">
         <v>316</v>
@@ -3815,10 +3806,10 @@
         <v>47947</v>
       </c>
       <c r="T18" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="U18" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="V18" t="s">
         <v>156</v>
@@ -3830,13 +3821,13 @@
         <v>47968</v>
       </c>
       <c r="Y18" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="Z18" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="AA18" t="s">
-        <v>375</v>
+        <v>42</v>
       </c>
       <c r="AB18" s="2">
         <v>45337</v>
@@ -3847,31 +3838,31 @@
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="B19" s="2">
         <v>37666</v>
       </c>
       <c r="C19" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D19" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="E19" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="F19">
         <v>13</v>
       </c>
       <c r="G19" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="H19">
         <v>15000</v>
       </c>
       <c r="I19" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="J19">
         <v>819012345</v>
@@ -3880,7 +3871,7 @@
         <v>44</v>
       </c>
       <c r="L19" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="M19" t="s">
         <v>31</v>
@@ -3889,13 +3880,13 @@
         <v>819099999</v>
       </c>
       <c r="O19" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="P19" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="Q19" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="R19" s="2">
         <v>44640</v>
@@ -3904,10 +3895,10 @@
         <v>48292</v>
       </c>
       <c r="T19" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="U19" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="V19" t="s">
         <v>164</v>
@@ -3919,13 +3910,13 @@
         <v>48304</v>
       </c>
       <c r="Y19" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="Z19" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="AA19" t="s">
-        <v>320</v>
+        <v>46</v>
       </c>
       <c r="AB19" s="2">
         <v>45352</v>
@@ -3936,7 +3927,7 @@
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="B20" s="2">
         <v>37174</v>
@@ -3945,22 +3936,22 @@
         <v>307</v>
       </c>
       <c r="D20" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="E20" t="s">
         <v>309</v>
       </c>
       <c r="F20" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="G20" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="H20">
         <v>462016</v>
       </c>
       <c r="I20" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="J20">
         <v>9425012345</v>
@@ -3969,7 +3960,7 @@
         <v>56</v>
       </c>
       <c r="L20" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="M20" t="s">
         <v>31</v>
@@ -3978,10 +3969,10 @@
         <v>9425099112</v>
       </c>
       <c r="O20" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="P20" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="Q20" t="s">
         <v>316</v>
@@ -3993,10 +3984,10 @@
         <v>47617</v>
       </c>
       <c r="T20" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="U20" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="V20" t="s">
         <v>156</v>
@@ -4008,13 +3999,13 @@
         <v>47634</v>
       </c>
       <c r="Y20" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="Z20" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="AA20" t="s">
-        <v>320</v>
+        <v>50</v>
       </c>
       <c r="AB20" s="2">
         <v>45306</v>
@@ -4025,31 +4016,31 @@
     </row>
     <row r="21" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="B21" s="2">
         <v>37498</v>
       </c>
       <c r="C21" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D21" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="E21" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="F21" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="G21" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="H21">
         <v>28001</v>
       </c>
       <c r="I21" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="J21">
         <v>346001234</v>
@@ -4058,7 +4049,7 @@
         <v>30</v>
       </c>
       <c r="L21" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="M21" t="s">
         <v>31</v>
@@ -4067,13 +4058,13 @@
         <v>346009999</v>
       </c>
       <c r="O21" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="P21" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="Q21" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="R21" s="2">
         <v>44451</v>
@@ -4082,10 +4073,10 @@
         <v>48102</v>
       </c>
       <c r="T21" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="U21" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="V21" t="s">
         <v>262</v>
@@ -4097,13 +4088,13 @@
         <v>48121</v>
       </c>
       <c r="Y21" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="Z21" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="AA21" t="s">
-        <v>320</v>
+        <v>54</v>
       </c>
       <c r="AB21" s="2">
         <v>45332</v>
@@ -4114,7 +4105,7 @@
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="B22" s="2">
         <v>37340</v>
@@ -4123,22 +4114,22 @@
         <v>307</v>
       </c>
       <c r="D22" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="E22" t="s">
         <v>309</v>
       </c>
       <c r="F22" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="G22" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="H22">
         <v>560038</v>
       </c>
       <c r="I22" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="J22">
         <v>9845012345</v>
@@ -4147,7 +4138,7 @@
         <v>40</v>
       </c>
       <c r="L22" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="M22" t="s">
         <v>31</v>
@@ -4156,10 +4147,10 @@
         <v>9845011223</v>
       </c>
       <c r="O22" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="P22" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="Q22" t="s">
         <v>316</v>
@@ -4171,10 +4162,10 @@
         <v>47867</v>
       </c>
       <c r="T22" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="U22" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="V22" t="s">
         <v>156</v>
@@ -4186,13 +4177,13 @@
         <v>47879</v>
       </c>
       <c r="Y22" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="Z22" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="AA22" t="s">
-        <v>349</v>
+        <v>58</v>
       </c>
       <c r="AB22" s="2">
         <v>45306</v>
@@ -4203,7 +4194,7 @@
     </row>
     <row r="23" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="B23" s="2">
         <v>37746</v>
@@ -4212,22 +4203,22 @@
         <v>307</v>
       </c>
       <c r="D23" t="s">
+        <v>556</v>
+      </c>
+      <c r="E23" t="s">
+        <v>557</v>
+      </c>
+      <c r="F23" t="s">
+        <v>558</v>
+      </c>
+      <c r="G23" t="s">
         <v>559</v>
-      </c>
-      <c r="E23" t="s">
-        <v>560</v>
-      </c>
-      <c r="F23" t="s">
-        <v>561</v>
-      </c>
-      <c r="G23" t="s">
-        <v>562</v>
       </c>
       <c r="H23">
         <v>1311</v>
       </c>
       <c r="I23" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="J23">
         <v>551191234</v>
@@ -4236,7 +4227,7 @@
         <v>48</v>
       </c>
       <c r="L23" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="M23" t="s">
         <v>36</v>
@@ -4245,13 +4236,13 @@
         <v>551199999</v>
       </c>
       <c r="O23" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="P23" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="Q23" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="R23" s="2">
         <v>44788</v>
@@ -4260,10 +4251,10 @@
         <v>48440</v>
       </c>
       <c r="T23" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="U23" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="V23" t="s">
         <v>86</v>
@@ -4275,13 +4266,13 @@
         <v>48457</v>
       </c>
       <c r="Y23" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="Z23" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="AA23" t="s">
-        <v>320</v>
+        <v>32</v>
       </c>
       <c r="AB23" s="2">
         <v>45371</v>
@@ -4292,7 +4283,7 @@
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="B24" s="2">
         <v>36993</v>
@@ -4301,7 +4292,7 @@
         <v>307</v>
       </c>
       <c r="D24" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="E24" t="s">
         <v>309</v>
@@ -4310,13 +4301,13 @@
         <v>310</v>
       </c>
       <c r="G24" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="H24">
         <v>440022</v>
       </c>
       <c r="I24" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="J24">
         <v>9422012345</v>
@@ -4325,7 +4316,7 @@
         <v>56</v>
       </c>
       <c r="L24" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="M24" t="s">
         <v>31</v>
@@ -4334,10 +4325,10 @@
         <v>9422099881</v>
       </c>
       <c r="O24" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="P24" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="Q24" t="s">
         <v>316</v>
@@ -4349,10 +4340,10 @@
         <v>47673</v>
       </c>
       <c r="T24" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="U24" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="V24" t="s">
         <v>156</v>
@@ -4364,13 +4355,13 @@
         <v>47695</v>
       </c>
       <c r="Y24" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="Z24" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="AA24" t="s">
-        <v>320</v>
+        <v>37</v>
       </c>
       <c r="AB24" s="2">
         <v>45306</v>
@@ -4381,7 +4372,7 @@
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="B25" s="2">
         <v>37571</v>
@@ -4390,22 +4381,22 @@
         <v>307</v>
       </c>
       <c r="D25" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="E25" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="F25">
         <v>11</v>
       </c>
       <c r="G25" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="H25">
         <v>6000</v>
       </c>
       <c r="I25" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="J25">
         <v>821012345</v>
@@ -4414,7 +4405,7 @@
         <v>35</v>
       </c>
       <c r="L25" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="M25" t="s">
         <v>31</v>
@@ -4423,13 +4414,13 @@
         <v>821099999</v>
       </c>
       <c r="O25" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="P25" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="Q25" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="R25" s="2">
         <v>44535</v>
@@ -4438,13 +4429,13 @@
         <v>48186</v>
       </c>
       <c r="T25" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="U25" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="V25" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="W25" s="2">
         <v>44571</v>
@@ -4453,13 +4444,13 @@
         <v>48213</v>
       </c>
       <c r="Y25" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="Z25" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="AA25" t="s">
-        <v>320</v>
+        <v>42</v>
       </c>
       <c r="AB25" s="2">
         <v>45337</v>
@@ -4470,7 +4461,7 @@
     </row>
     <row r="26" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="B26" s="2">
         <v>37802</v>
@@ -4479,22 +4470,22 @@
         <v>307</v>
       </c>
       <c r="D26" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="E26" t="s">
         <v>309</v>
       </c>
       <c r="F26" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="G26" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="H26">
         <v>800001</v>
       </c>
       <c r="I26" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="J26">
         <v>9431012345</v>
@@ -4503,7 +4494,7 @@
         <v>40</v>
       </c>
       <c r="L26" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="M26" t="s">
         <v>31</v>
@@ -4512,10 +4503,10 @@
         <v>9431099887</v>
       </c>
       <c r="O26" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="P26" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="Q26" t="s">
         <v>316</v>
@@ -4527,10 +4518,10 @@
         <v>48501</v>
       </c>
       <c r="T26" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="U26" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="V26" t="s">
         <v>156</v>
@@ -4542,13 +4533,13 @@
         <v>48518</v>
       </c>
       <c r="Y26" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="Z26" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="AA26" t="s">
-        <v>349</v>
+        <v>46</v>
       </c>
       <c r="AB26" s="2">
         <v>45383</v>

</xml_diff>